<commit_message>
Correcoes nos docs e na pagina de funcionario
</commit_message>
<xml_diff>
--- a/docs/Planejamento/Estimativa por Pontos de Casos de Uso Projeto Avaliador de Desempenho Vrs 1.0.xlsx
+++ b/docs/Planejamento/Estimativa por Pontos de Casos de Uso Projeto Avaliador de Desempenho Vrs 1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José\Desktop\Finais - Organização por favor\docs\Planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FAITEC\ADD\Finais\docs\Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1983E3-0F2D-4052-957F-F8CA72BE2A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE67D86-2210-4034-8B40-2FDAA3868989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,9 +393,6 @@
     <t>Funcionário</t>
   </si>
   <si>
-    <t>Aplicador de Avaliação</t>
-  </si>
-  <si>
     <t>Editar Perfil</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>Responder</t>
+  </si>
+  <si>
+    <t>Avaliador</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1094,58 +1094,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1157,27 +1144,78 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1186,84 +1224,49 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1742,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U127"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A100" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="H116" sqref="H116"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A88" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1762,17 +1765,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="114"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="95"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="66"/>
@@ -1789,11 +1792,11 @@
       <c r="A3" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="112"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="93"/>
       <c r="E3" s="59"/>
       <c r="F3" s="59"/>
       <c r="G3" s="59"/>
@@ -1944,17 +1947,17 @@
       <c r="I14" s="39"/>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="130" t="s">
+      <c r="A15" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="130"/>
-      <c r="C15" s="130"/>
-      <c r="D15" s="130"/>
-      <c r="E15" s="130"/>
-      <c r="F15" s="130"/>
-      <c r="G15" s="130"/>
-      <c r="H15" s="130"/>
-      <c r="I15" s="130"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
@@ -1963,12 +1966,12 @@
       <c r="B16" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
       <c r="I16" s="40" t="s">
         <v>2</v>
       </c>
@@ -1977,7 +1980,7 @@
       <c r="A17" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="132" t="s">
+      <c r="B17" s="75" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="71"/>
@@ -1994,7 +1997,7 @@
       <c r="A18" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="132" t="s">
+      <c r="B18" s="75" t="s">
         <v>104</v>
       </c>
       <c r="C18" s="71"/>
@@ -2050,46 +2053,46 @@
       <c r="A21" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="98"/>
+      <c r="C21" s="86"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="B22" s="117">
+      <c r="B22" s="76">
         <v>1</v>
       </c>
-      <c r="C22" s="118"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="B23" s="117">
+      <c r="A23" s="134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="76">
         <v>2</v>
       </c>
-      <c r="C23" s="118"/>
+      <c r="C23" s="77"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="117"/>
-      <c r="C24" s="118"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="77"/>
     </row>
     <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="128">
+      <c r="B25" s="79">
         <f>SUM(B22:C24)</f>
         <v>3</v>
       </c>
-      <c r="C25" s="129"/>
+      <c r="C25" s="80"/>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
@@ -2115,12 +2118,12 @@
       <c r="B28" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="133"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="133"/>
-      <c r="H28" s="133"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
       <c r="I28" s="40" t="s">
         <v>2</v>
       </c>
@@ -2191,10 +2194,10 @@
       <c r="A33" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="96" t="s">
+      <c r="B33" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="98"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="H33" s="3"/>
@@ -2205,12 +2208,12 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="74">
+        <v>119</v>
+      </c>
+      <c r="B34" s="81">
         <v>5</v>
       </c>
-      <c r="C34" s="126"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -2221,12 +2224,12 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="69" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="74">
+        <v>120</v>
+      </c>
+      <c r="B35" s="81">
         <v>5</v>
       </c>
-      <c r="C35" s="75"/>
+      <c r="C35" s="90"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -2234,12 +2237,12 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="B36" s="74">
+        <v>121</v>
+      </c>
+      <c r="B36" s="81">
         <v>5</v>
       </c>
-      <c r="C36" s="75"/>
+      <c r="C36" s="90"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -2247,12 +2250,12 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="B37" s="74">
+        <v>122</v>
+      </c>
+      <c r="B37" s="81">
         <v>5</v>
       </c>
-      <c r="C37" s="75"/>
+      <c r="C37" s="90"/>
       <c r="D37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -2260,12 +2263,12 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" s="74">
+        <v>123</v>
+      </c>
+      <c r="B38" s="81">
         <v>5</v>
       </c>
-      <c r="C38" s="75"/>
+      <c r="C38" s="90"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -2273,12 +2276,12 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="69" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="74">
+        <v>124</v>
+      </c>
+      <c r="B39" s="81">
         <v>10</v>
       </c>
-      <c r="C39" s="75"/>
+      <c r="C39" s="90"/>
       <c r="D39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -2286,12 +2289,12 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="69" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="74">
+        <v>125</v>
+      </c>
+      <c r="B40" s="81">
         <v>5</v>
       </c>
-      <c r="C40" s="75"/>
+      <c r="C40" s="90"/>
       <c r="D40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -2299,12 +2302,12 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="69" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="74">
+        <v>126</v>
+      </c>
+      <c r="B41" s="81">
         <v>10</v>
       </c>
-      <c r="C41" s="75"/>
+      <c r="C41" s="90"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -2312,12 +2315,12 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="74">
+        <v>127</v>
+      </c>
+      <c r="B42" s="81">
         <v>5</v>
       </c>
-      <c r="C42" s="75"/>
+      <c r="C42" s="90"/>
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -2325,12 +2328,12 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="B43" s="74">
+        <v>128</v>
+      </c>
+      <c r="B43" s="81">
         <v>5</v>
       </c>
-      <c r="C43" s="75"/>
+      <c r="C43" s="90"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -2338,12 +2341,12 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" s="74">
+        <v>129</v>
+      </c>
+      <c r="B44" s="81">
         <v>5</v>
       </c>
-      <c r="C44" s="75"/>
+      <c r="C44" s="90"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -2351,12 +2354,12 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="B45" s="74">
+        <v>130</v>
+      </c>
+      <c r="B45" s="81">
         <v>5</v>
       </c>
-      <c r="C45" s="75"/>
+      <c r="C45" s="90"/>
       <c r="D45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -2364,12 +2367,12 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="68" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" s="74">
+        <v>131</v>
+      </c>
+      <c r="B46" s="81">
         <v>5</v>
       </c>
-      <c r="C46" s="126"/>
+      <c r="C46" s="82"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -2379,12 +2382,12 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="57" t="s">
-        <v>133</v>
-      </c>
-      <c r="B47" s="74">
+        <v>132</v>
+      </c>
+      <c r="B47" s="81">
         <v>5</v>
       </c>
-      <c r="C47" s="126"/>
+      <c r="C47" s="82"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -2393,11 +2396,11 @@
       <c r="A48" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="115">
+      <c r="B48" s="96">
         <f>SUM(B34:B47)</f>
         <v>80</v>
       </c>
-      <c r="C48" s="116"/>
+      <c r="C48" s="97"/>
       <c r="D48" s="3" t="s">
         <v>14</v>
       </c>
@@ -2422,11 +2425,11 @@
       <c r="A50" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="128">
+      <c r="B50" s="79">
         <f>B25+B48</f>
         <v>83</v>
       </c>
-      <c r="C50" s="129"/>
+      <c r="C50" s="80"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
@@ -2451,17 +2454,17 @@
       <c r="U51" s="9"/>
     </row>
     <row r="52" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="96" t="s">
+      <c r="A52" s="84" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="97"/>
-      <c r="C52" s="97"/>
-      <c r="D52" s="97"/>
-      <c r="E52" s="97"/>
-      <c r="F52" s="97"/>
-      <c r="G52" s="97"/>
-      <c r="H52" s="97"/>
-      <c r="I52" s="98"/>
+      <c r="B52" s="85"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="85"/>
+      <c r="H52" s="85"/>
+      <c r="I52" s="86"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
@@ -2475,17 +2478,17 @@
       <c r="U52" s="9"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A53" s="90" t="s">
+      <c r="A53" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="91"/>
-      <c r="C53" s="91"/>
-      <c r="D53" s="91"/>
-      <c r="E53" s="91"/>
-      <c r="F53" s="91"/>
-      <c r="G53" s="91"/>
-      <c r="H53" s="91"/>
-      <c r="I53" s="92"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="88"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="88"/>
+      <c r="F53" s="88"/>
+      <c r="G53" s="88"/>
+      <c r="H53" s="88"/>
+      <c r="I53" s="89"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
@@ -2499,17 +2502,17 @@
       <c r="U53" s="9"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A54" s="90" t="s">
+      <c r="A54" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="91"/>
-      <c r="C54" s="91"/>
-      <c r="D54" s="91"/>
-      <c r="E54" s="91"/>
-      <c r="F54" s="91"/>
-      <c r="G54" s="91"/>
-      <c r="H54" s="91"/>
-      <c r="I54" s="92"/>
+      <c r="B54" s="88"/>
+      <c r="C54" s="88"/>
+      <c r="D54" s="88"/>
+      <c r="E54" s="88"/>
+      <c r="F54" s="88"/>
+      <c r="G54" s="88"/>
+      <c r="H54" s="88"/>
+      <c r="I54" s="89"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
@@ -2523,17 +2526,17 @@
       <c r="U54" s="9"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A55" s="90" t="s">
+      <c r="A55" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="B55" s="91"/>
-      <c r="C55" s="91"/>
-      <c r="D55" s="91"/>
-      <c r="E55" s="91"/>
-      <c r="F55" s="91"/>
-      <c r="G55" s="91"/>
-      <c r="H55" s="91"/>
-      <c r="I55" s="92"/>
+      <c r="B55" s="88"/>
+      <c r="C55" s="88"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="88"/>
+      <c r="F55" s="88"/>
+      <c r="G55" s="88"/>
+      <c r="H55" s="88"/>
+      <c r="I55" s="89"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -2547,17 +2550,17 @@
       <c r="U55" s="9"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A56" s="90" t="s">
+      <c r="A56" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="91"/>
-      <c r="C56" s="91"/>
-      <c r="D56" s="91"/>
-      <c r="E56" s="91"/>
-      <c r="F56" s="91"/>
-      <c r="G56" s="91"/>
-      <c r="H56" s="91"/>
-      <c r="I56" s="92"/>
+      <c r="B56" s="88"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="88"/>
+      <c r="E56" s="88"/>
+      <c r="F56" s="88"/>
+      <c r="G56" s="88"/>
+      <c r="H56" s="88"/>
+      <c r="I56" s="89"/>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
@@ -2574,12 +2577,12 @@
       <c r="A57" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B57" s="127" t="s">
+      <c r="B57" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="127"/>
-      <c r="D57" s="127"/>
-      <c r="E57" s="127"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="83"/>
+      <c r="E57" s="83"/>
       <c r="F57" s="46" t="s">
         <v>2</v>
       </c>
@@ -2618,11 +2621,11 @@
       <c r="G58" s="55">
         <v>4</v>
       </c>
-      <c r="H58" s="72">
+      <c r="H58" s="106">
         <f t="shared" ref="H58:H70" si="0">F58*G58</f>
         <v>8</v>
       </c>
-      <c r="I58" s="72"/>
+      <c r="I58" s="106"/>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
@@ -2651,11 +2654,11 @@
       <c r="G59" s="55">
         <v>0</v>
       </c>
-      <c r="H59" s="72">
+      <c r="H59" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I59" s="72"/>
+      <c r="I59" s="106"/>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
@@ -2684,11 +2687,11 @@
       <c r="G60" s="55">
         <v>0</v>
       </c>
-      <c r="H60" s="72">
+      <c r="H60" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I60" s="72"/>
+      <c r="I60" s="106"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -2717,11 +2720,11 @@
       <c r="G61" s="55">
         <v>0</v>
       </c>
-      <c r="H61" s="72">
+      <c r="H61" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I61" s="72"/>
+      <c r="I61" s="106"/>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
@@ -2750,11 +2753,11 @@
       <c r="G62" s="55">
         <v>0</v>
       </c>
-      <c r="H62" s="72">
+      <c r="H62" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I62" s="72"/>
+      <c r="I62" s="106"/>
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="M62" s="11"/>
@@ -2783,11 +2786,11 @@
       <c r="G63" s="55">
         <v>0</v>
       </c>
-      <c r="H63" s="72">
+      <c r="H63" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I63" s="72"/>
+      <c r="I63" s="106"/>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
@@ -2816,11 +2819,11 @@
       <c r="G64" s="55">
         <v>0</v>
       </c>
-      <c r="H64" s="72">
+      <c r="H64" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I64" s="72"/>
+      <c r="I64" s="106"/>
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
@@ -2849,11 +2852,11 @@
       <c r="G65" s="55">
         <v>0</v>
       </c>
-      <c r="H65" s="72">
+      <c r="H65" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I65" s="72"/>
+      <c r="I65" s="106"/>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
@@ -2882,11 +2885,11 @@
       <c r="G66" s="55">
         <v>0</v>
       </c>
-      <c r="H66" s="72">
+      <c r="H66" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I66" s="72"/>
+      <c r="I66" s="106"/>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
@@ -2915,11 +2918,11 @@
       <c r="G67" s="55">
         <v>0</v>
       </c>
-      <c r="H67" s="72">
+      <c r="H67" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I67" s="72"/>
+      <c r="I67" s="106"/>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
@@ -2948,11 +2951,11 @@
       <c r="G68" s="55">
         <v>0</v>
       </c>
-      <c r="H68" s="72">
+      <c r="H68" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I68" s="72"/>
+      <c r="I68" s="106"/>
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
@@ -2981,11 +2984,11 @@
       <c r="G69" s="55">
         <v>3</v>
       </c>
-      <c r="H69" s="72">
+      <c r="H69" s="106">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I69" s="72"/>
+      <c r="I69" s="106"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
@@ -3014,11 +3017,11 @@
       <c r="G70" s="55">
         <v>2</v>
       </c>
-      <c r="H70" s="72">
+      <c r="H70" s="106">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I70" s="72"/>
+      <c r="I70" s="106"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
@@ -3032,20 +3035,20 @@
       <c r="U70" s="9"/>
     </row>
     <row r="71" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="88" t="s">
+      <c r="A71" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="80"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="80"/>
-      <c r="E71" s="80"/>
-      <c r="F71" s="80"/>
-      <c r="G71" s="89"/>
-      <c r="H71" s="125">
+      <c r="B71" s="108"/>
+      <c r="C71" s="108"/>
+      <c r="D71" s="108"/>
+      <c r="E71" s="108"/>
+      <c r="F71" s="108"/>
+      <c r="G71" s="109"/>
+      <c r="H71" s="110">
         <f>0.6+(0.01*(SUM(H58:I70)))</f>
         <v>0.73</v>
       </c>
-      <c r="I71" s="125"/>
+      <c r="I71" s="110"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
@@ -3080,17 +3083,17 @@
       <c r="U72" s="9"/>
     </row>
     <row r="73" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="96" t="s">
+      <c r="A73" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="97"/>
-      <c r="C73" s="97"/>
-      <c r="D73" s="97"/>
-      <c r="E73" s="97"/>
-      <c r="F73" s="97"/>
-      <c r="G73" s="97"/>
-      <c r="H73" s="97"/>
-      <c r="I73" s="98"/>
+      <c r="B73" s="85"/>
+      <c r="C73" s="85"/>
+      <c r="D73" s="85"/>
+      <c r="E73" s="85"/>
+      <c r="F73" s="85"/>
+      <c r="G73" s="85"/>
+      <c r="H73" s="85"/>
+      <c r="I73" s="86"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -3104,17 +3107,17 @@
       <c r="U73" s="9"/>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A74" s="90" t="s">
+      <c r="A74" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B74" s="91"/>
-      <c r="C74" s="91"/>
-      <c r="D74" s="91"/>
-      <c r="E74" s="91"/>
-      <c r="F74" s="91"/>
-      <c r="G74" s="91"/>
-      <c r="H74" s="91"/>
-      <c r="I74" s="92"/>
+      <c r="B74" s="88"/>
+      <c r="C74" s="88"/>
+      <c r="D74" s="88"/>
+      <c r="E74" s="88"/>
+      <c r="F74" s="88"/>
+      <c r="G74" s="88"/>
+      <c r="H74" s="88"/>
+      <c r="I74" s="89"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
@@ -3128,17 +3131,17 @@
       <c r="U74" s="9"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A75" s="90" t="s">
+      <c r="A75" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="91"/>
-      <c r="C75" s="91"/>
-      <c r="D75" s="91"/>
-      <c r="E75" s="91"/>
-      <c r="F75" s="91"/>
-      <c r="G75" s="91"/>
-      <c r="H75" s="91"/>
-      <c r="I75" s="92"/>
+      <c r="B75" s="88"/>
+      <c r="C75" s="88"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="88"/>
+      <c r="F75" s="88"/>
+      <c r="G75" s="88"/>
+      <c r="H75" s="88"/>
+      <c r="I75" s="89"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -3152,17 +3155,17 @@
       <c r="U75" s="9"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A76" s="90" t="s">
+      <c r="A76" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="91"/>
-      <c r="C76" s="91"/>
-      <c r="D76" s="91"/>
-      <c r="E76" s="91"/>
-      <c r="F76" s="91"/>
-      <c r="G76" s="91"/>
-      <c r="H76" s="91"/>
-      <c r="I76" s="92"/>
+      <c r="B76" s="88"/>
+      <c r="C76" s="88"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="88"/>
+      <c r="F76" s="88"/>
+      <c r="G76" s="88"/>
+      <c r="H76" s="88"/>
+      <c r="I76" s="89"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
@@ -3176,17 +3179,17 @@
       <c r="U76" s="9"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A77" s="90" t="s">
+      <c r="A77" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="91"/>
-      <c r="F77" s="91"/>
-      <c r="G77" s="91"/>
-      <c r="H77" s="91"/>
-      <c r="I77" s="92"/>
+      <c r="B77" s="88"/>
+      <c r="C77" s="88"/>
+      <c r="D77" s="88"/>
+      <c r="E77" s="88"/>
+      <c r="F77" s="88"/>
+      <c r="G77" s="88"/>
+      <c r="H77" s="88"/>
+      <c r="I77" s="89"/>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
@@ -3200,17 +3203,17 @@
       <c r="U77" s="9"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A78" s="90" t="s">
+      <c r="A78" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="91"/>
-      <c r="C78" s="91"/>
-      <c r="D78" s="91"/>
-      <c r="E78" s="91"/>
-      <c r="F78" s="91"/>
-      <c r="G78" s="91"/>
-      <c r="H78" s="91"/>
-      <c r="I78" s="92"/>
+      <c r="B78" s="88"/>
+      <c r="C78" s="88"/>
+      <c r="D78" s="88"/>
+      <c r="E78" s="88"/>
+      <c r="F78" s="88"/>
+      <c r="G78" s="88"/>
+      <c r="H78" s="88"/>
+      <c r="I78" s="89"/>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
@@ -3227,13 +3230,13 @@
       <c r="A79" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B79" s="122" t="s">
+      <c r="B79" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C79" s="123"/>
-      <c r="D79" s="123"/>
-      <c r="E79" s="123"/>
-      <c r="F79" s="124"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="104"/>
+      <c r="E79" s="104"/>
+      <c r="F79" s="105"/>
       <c r="G79" s="46" t="s">
         <v>2</v>
       </c>
@@ -3259,13 +3262,13 @@
       <c r="A80" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B80" s="90" t="s">
+      <c r="B80" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="C80" s="91"/>
-      <c r="D80" s="91"/>
-      <c r="E80" s="91"/>
-      <c r="F80" s="92"/>
+      <c r="C80" s="88"/>
+      <c r="D80" s="88"/>
+      <c r="E80" s="88"/>
+      <c r="F80" s="89"/>
       <c r="G80" s="42">
         <v>1.5</v>
       </c>
@@ -3296,13 +3299,13 @@
       <c r="A81" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B81" s="90" t="s">
+      <c r="B81" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C81" s="91"/>
-      <c r="D81" s="91"/>
-      <c r="E81" s="91"/>
-      <c r="F81" s="92"/>
+      <c r="C81" s="88"/>
+      <c r="D81" s="88"/>
+      <c r="E81" s="88"/>
+      <c r="F81" s="89"/>
       <c r="G81" s="42">
         <v>0.5</v>
       </c>
@@ -3322,13 +3325,13 @@
       <c r="A82" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B82" s="90" t="s">
+      <c r="B82" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="C82" s="91"/>
-      <c r="D82" s="91"/>
-      <c r="E82" s="91"/>
-      <c r="F82" s="92"/>
+      <c r="C82" s="88"/>
+      <c r="D82" s="88"/>
+      <c r="E82" s="88"/>
+      <c r="F82" s="89"/>
       <c r="G82" s="42">
         <v>1</v>
       </c>
@@ -3348,13 +3351,13 @@
       <c r="A83" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B83" s="90" t="s">
+      <c r="B83" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="C83" s="91"/>
-      <c r="D83" s="91"/>
-      <c r="E83" s="91"/>
-      <c r="F83" s="92"/>
+      <c r="C83" s="88"/>
+      <c r="D83" s="88"/>
+      <c r="E83" s="88"/>
+      <c r="F83" s="89"/>
       <c r="G83" s="42">
         <v>0.5</v>
       </c>
@@ -3374,13 +3377,13 @@
       <c r="A84" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B84" s="90" t="s">
+      <c r="B84" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="C84" s="91"/>
-      <c r="D84" s="91"/>
-      <c r="E84" s="91"/>
-      <c r="F84" s="92"/>
+      <c r="C84" s="88"/>
+      <c r="D84" s="88"/>
+      <c r="E84" s="88"/>
+      <c r="F84" s="89"/>
       <c r="G84" s="42">
         <v>1</v>
       </c>
@@ -3400,13 +3403,13 @@
       <c r="A85" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B85" s="93" t="s">
+      <c r="B85" s="131" t="s">
         <v>100</v>
       </c>
-      <c r="C85" s="94"/>
-      <c r="D85" s="94"/>
-      <c r="E85" s="94"/>
-      <c r="F85" s="95"/>
+      <c r="C85" s="132"/>
+      <c r="D85" s="132"/>
+      <c r="E85" s="132"/>
+      <c r="F85" s="133"/>
       <c r="G85" s="42">
         <v>2</v>
       </c>
@@ -3426,13 +3429,13 @@
       <c r="A86" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B86" s="90" t="s">
+      <c r="B86" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C86" s="91"/>
-      <c r="D86" s="91"/>
-      <c r="E86" s="91"/>
-      <c r="F86" s="92"/>
+      <c r="C86" s="88"/>
+      <c r="D86" s="88"/>
+      <c r="E86" s="88"/>
+      <c r="F86" s="89"/>
       <c r="G86" s="42">
         <v>-1</v>
       </c>
@@ -3452,13 +3455,13 @@
       <c r="A87" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="B87" s="90" t="s">
+      <c r="B87" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C87" s="91"/>
-      <c r="D87" s="91"/>
-      <c r="E87" s="91"/>
-      <c r="F87" s="92"/>
+      <c r="C87" s="88"/>
+      <c r="D87" s="88"/>
+      <c r="E87" s="88"/>
+      <c r="F87" s="89"/>
       <c r="G87" s="42">
         <v>-1</v>
       </c>
@@ -3475,16 +3478,16 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="88" t="s">
+      <c r="A88" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="80"/>
-      <c r="C88" s="80"/>
-      <c r="D88" s="80"/>
-      <c r="E88" s="80"/>
-      <c r="F88" s="80"/>
-      <c r="G88" s="80"/>
-      <c r="H88" s="89"/>
+      <c r="B88" s="108"/>
+      <c r="C88" s="108"/>
+      <c r="D88" s="108"/>
+      <c r="E88" s="108"/>
+      <c r="F88" s="108"/>
+      <c r="G88" s="108"/>
+      <c r="H88" s="109"/>
       <c r="I88" s="18">
         <f>1.4+(-0.03*(SUM(I80:I87)))</f>
         <v>1.04</v>
@@ -3504,197 +3507,197 @@
       <c r="B91" s="13"/>
     </row>
     <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="85" t="s">
+      <c r="A92" s="128" t="s">
         <v>108</v>
       </c>
-      <c r="B92" s="86"/>
-      <c r="C92" s="86"/>
-      <c r="D92" s="86"/>
-      <c r="E92" s="86"/>
-      <c r="F92" s="86"/>
-      <c r="G92" s="86"/>
-      <c r="H92" s="86"/>
-      <c r="I92" s="87"/>
+      <c r="B92" s="129"/>
+      <c r="C92" s="129"/>
+      <c r="D92" s="129"/>
+      <c r="E92" s="129"/>
+      <c r="F92" s="129"/>
+      <c r="G92" s="129"/>
+      <c r="H92" s="129"/>
+      <c r="I92" s="130"/>
     </row>
     <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="82" t="s">
+      <c r="A93" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="B93" s="83"/>
-      <c r="C93" s="83"/>
-      <c r="D93" s="83"/>
-      <c r="E93" s="83"/>
-      <c r="F93" s="83"/>
-      <c r="G93" s="83"/>
-      <c r="H93" s="83"/>
-      <c r="I93" s="84"/>
+      <c r="B93" s="126"/>
+      <c r="C93" s="126"/>
+      <c r="D93" s="126"/>
+      <c r="E93" s="126"/>
+      <c r="F93" s="126"/>
+      <c r="G93" s="126"/>
+      <c r="H93" s="126"/>
+      <c r="I93" s="127"/>
     </row>
     <row r="94" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="79" t="s">
+      <c r="A94" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="B94" s="80"/>
-      <c r="C94" s="80"/>
-      <c r="D94" s="80"/>
-      <c r="E94" s="80"/>
-      <c r="F94" s="80"/>
-      <c r="G94" s="80"/>
-      <c r="H94" s="80"/>
-      <c r="I94" s="81"/>
+      <c r="B94" s="108"/>
+      <c r="C94" s="108"/>
+      <c r="D94" s="108"/>
+      <c r="E94" s="108"/>
+      <c r="F94" s="108"/>
+      <c r="G94" s="108"/>
+      <c r="H94" s="108"/>
+      <c r="I94" s="115"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" s="119" t="s">
+      <c r="A95" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="B95" s="120"/>
-      <c r="C95" s="120"/>
-      <c r="D95" s="120"/>
-      <c r="E95" s="120"/>
-      <c r="F95" s="120"/>
-      <c r="G95" s="120"/>
-      <c r="H95" s="120"/>
-      <c r="I95" s="121"/>
+      <c r="B95" s="99"/>
+      <c r="C95" s="99"/>
+      <c r="D95" s="99"/>
+      <c r="E95" s="99"/>
+      <c r="F95" s="99"/>
+      <c r="G95" s="99"/>
+      <c r="H95" s="99"/>
+      <c r="I95" s="100"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" s="119" t="s">
+      <c r="A96" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="B96" s="120"/>
-      <c r="C96" s="120"/>
-      <c r="D96" s="120"/>
-      <c r="E96" s="120"/>
-      <c r="F96" s="120"/>
-      <c r="G96" s="120"/>
-      <c r="H96" s="120"/>
-      <c r="I96" s="121"/>
+      <c r="B96" s="99"/>
+      <c r="C96" s="99"/>
+      <c r="D96" s="99"/>
+      <c r="E96" s="99"/>
+      <c r="F96" s="99"/>
+      <c r="G96" s="99"/>
+      <c r="H96" s="99"/>
+      <c r="I96" s="100"/>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="76"/>
-      <c r="B97" s="77"/>
-      <c r="C97" s="77"/>
-      <c r="D97" s="77"/>
-      <c r="E97" s="77"/>
-      <c r="F97" s="78"/>
-      <c r="G97" s="108" t="s">
+      <c r="A97" s="119"/>
+      <c r="B97" s="120"/>
+      <c r="C97" s="120"/>
+      <c r="D97" s="120"/>
+      <c r="E97" s="120"/>
+      <c r="F97" s="121"/>
+      <c r="G97" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="H97" s="109"/>
+      <c r="H97" s="102"/>
       <c r="I97" s="20">
         <f>SUM(J80:J85)</f>
         <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="76"/>
-      <c r="B98" s="77"/>
-      <c r="C98" s="77"/>
-      <c r="D98" s="77"/>
-      <c r="E98" s="77"/>
-      <c r="F98" s="78"/>
-      <c r="G98" s="108" t="s">
+      <c r="A98" s="119"/>
+      <c r="B98" s="120"/>
+      <c r="C98" s="120"/>
+      <c r="D98" s="120"/>
+      <c r="E98" s="120"/>
+      <c r="F98" s="121"/>
+      <c r="G98" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="H98" s="109"/>
+      <c r="H98" s="102"/>
       <c r="I98" s="20">
         <f>SUM(J86:J87)</f>
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="76"/>
-      <c r="B99" s="77"/>
-      <c r="C99" s="77"/>
-      <c r="D99" s="77"/>
-      <c r="E99" s="77"/>
-      <c r="F99" s="78"/>
-      <c r="G99" s="108" t="s">
+      <c r="A99" s="119"/>
+      <c r="B99" s="120"/>
+      <c r="C99" s="120"/>
+      <c r="D99" s="120"/>
+      <c r="E99" s="120"/>
+      <c r="F99" s="121"/>
+      <c r="G99" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="H99" s="109"/>
+      <c r="H99" s="102"/>
       <c r="I99" s="20">
         <f>I97+I98</f>
         <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="102" t="s">
+      <c r="A100" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="B100" s="103"/>
-      <c r="C100" s="103"/>
-      <c r="D100" s="103"/>
-      <c r="E100" s="103"/>
-      <c r="F100" s="103"/>
-      <c r="G100" s="103"/>
-      <c r="H100" s="104"/>
+      <c r="B100" s="117"/>
+      <c r="C100" s="117"/>
+      <c r="D100" s="117"/>
+      <c r="E100" s="117"/>
+      <c r="F100" s="117"/>
+      <c r="G100" s="117"/>
+      <c r="H100" s="118"/>
       <c r="I100" s="21" t="str">
         <f>C111</f>
         <v>Reduzir a complexidade</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="79" t="s">
+      <c r="A101" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="B101" s="80"/>
-      <c r="C101" s="80"/>
-      <c r="D101" s="80"/>
-      <c r="E101" s="80"/>
-      <c r="F101" s="80"/>
-      <c r="G101" s="80"/>
-      <c r="H101" s="80"/>
-      <c r="I101" s="81"/>
+      <c r="B101" s="108"/>
+      <c r="C101" s="108"/>
+      <c r="D101" s="108"/>
+      <c r="E101" s="108"/>
+      <c r="F101" s="108"/>
+      <c r="G101" s="108"/>
+      <c r="H101" s="108"/>
+      <c r="I101" s="115"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="99" t="s">
+      <c r="A102" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B102" s="100"/>
-      <c r="C102" s="100"/>
-      <c r="D102" s="100"/>
-      <c r="E102" s="100"/>
-      <c r="F102" s="100"/>
-      <c r="G102" s="100"/>
-      <c r="H102" s="100"/>
-      <c r="I102" s="101"/>
+      <c r="B102" s="112"/>
+      <c r="C102" s="112"/>
+      <c r="D102" s="112"/>
+      <c r="E102" s="112"/>
+      <c r="F102" s="112"/>
+      <c r="G102" s="112"/>
+      <c r="H102" s="112"/>
+      <c r="I102" s="113"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103" s="99" t="s">
+      <c r="A103" s="111" t="s">
         <v>98</v>
       </c>
-      <c r="B103" s="100"/>
-      <c r="C103" s="100"/>
-      <c r="D103" s="100"/>
-      <c r="E103" s="100"/>
-      <c r="F103" s="100"/>
-      <c r="G103" s="100"/>
-      <c r="H103" s="100"/>
-      <c r="I103" s="101"/>
+      <c r="B103" s="112"/>
+      <c r="C103" s="112"/>
+      <c r="D103" s="112"/>
+      <c r="E103" s="112"/>
+      <c r="F103" s="112"/>
+      <c r="G103" s="112"/>
+      <c r="H103" s="112"/>
+      <c r="I103" s="113"/>
     </row>
     <row r="104" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="105" t="s">
+      <c r="A104" s="122" t="s">
         <v>99</v>
       </c>
-      <c r="B104" s="106"/>
-      <c r="C104" s="106"/>
-      <c r="D104" s="106"/>
-      <c r="E104" s="106"/>
-      <c r="F104" s="106"/>
-      <c r="G104" s="106"/>
-      <c r="H104" s="106"/>
-      <c r="I104" s="107"/>
+      <c r="B104" s="123"/>
+      <c r="C104" s="123"/>
+      <c r="D104" s="123"/>
+      <c r="E104" s="123"/>
+      <c r="F104" s="123"/>
+      <c r="G104" s="123"/>
+      <c r="H104" s="123"/>
+      <c r="I104" s="124"/>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="96" t="s">
+      <c r="A109" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="B109" s="97"/>
-      <c r="C109" s="97"/>
-      <c r="D109" s="97"/>
-      <c r="E109" s="97"/>
-      <c r="F109" s="97"/>
-      <c r="G109" s="97"/>
-      <c r="H109" s="98"/>
+      <c r="B109" s="85"/>
+      <c r="C109" s="85"/>
+      <c r="D109" s="85"/>
+      <c r="E109" s="85"/>
+      <c r="F109" s="85"/>
+      <c r="G109" s="85"/>
+      <c r="H109" s="86"/>
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="46" t="s">
@@ -3784,16 +3787,16 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="88" t="s">
+      <c r="A114" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="B114" s="80"/>
-      <c r="C114" s="80"/>
-      <c r="D114" s="80"/>
-      <c r="E114" s="80"/>
-      <c r="F114" s="80"/>
-      <c r="G114" s="80"/>
-      <c r="H114" s="89"/>
+      <c r="B114" s="108"/>
+      <c r="C114" s="108"/>
+      <c r="D114" s="108"/>
+      <c r="E114" s="108"/>
+      <c r="F114" s="108"/>
+      <c r="G114" s="108"/>
+      <c r="H114" s="109"/>
     </row>
     <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="46" t="s">
@@ -3884,16 +3887,16 @@
       <c r="H118" s="3"/>
     </row>
     <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="88" t="s">
+      <c r="A119" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="B119" s="80"/>
-      <c r="C119" s="80"/>
-      <c r="D119" s="80"/>
-      <c r="E119" s="80"/>
-      <c r="F119" s="80"/>
-      <c r="G119" s="80"/>
-      <c r="H119" s="89"/>
+      <c r="B119" s="108"/>
+      <c r="C119" s="108"/>
+      <c r="D119" s="108"/>
+      <c r="E119" s="108"/>
+      <c r="F119" s="108"/>
+      <c r="G119" s="108"/>
+      <c r="H119" s="109"/>
     </row>
     <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="46" t="s">
@@ -3998,38 +4001,53 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A53:I53"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="A56:I56"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="A97:F97"/>
+    <mergeCell ref="A94:I94"/>
+    <mergeCell ref="A93:I93"/>
+    <mergeCell ref="A92:I92"/>
+    <mergeCell ref="A88:H88"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A77:I77"/>
+    <mergeCell ref="A76:I76"/>
+    <mergeCell ref="A75:I75"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="A74:I74"/>
+    <mergeCell ref="A73:I73"/>
+    <mergeCell ref="A102:I102"/>
+    <mergeCell ref="A101:I101"/>
+    <mergeCell ref="A100:H100"/>
+    <mergeCell ref="A99:F99"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="A114:H114"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A104:I104"/>
+    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="G98:H98"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B48:C48"/>
@@ -4054,54 +4072,39 @@
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="B65:E65"/>
     <mergeCell ref="H65:I65"/>
-    <mergeCell ref="A74:I74"/>
-    <mergeCell ref="A73:I73"/>
-    <mergeCell ref="A102:I102"/>
-    <mergeCell ref="A101:I101"/>
-    <mergeCell ref="A100:H100"/>
-    <mergeCell ref="A99:F99"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="A114:H114"/>
-    <mergeCell ref="A109:H109"/>
-    <mergeCell ref="A104:I104"/>
-    <mergeCell ref="A103:I103"/>
-    <mergeCell ref="G99:H99"/>
-    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="A53:I53"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="A97:F97"/>
-    <mergeCell ref="A94:I94"/>
-    <mergeCell ref="A93:I93"/>
-    <mergeCell ref="A92:I92"/>
-    <mergeCell ref="A88:H88"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="A77:I77"/>
-    <mergeCell ref="A76:I76"/>
-    <mergeCell ref="A75:I75"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B29:H29"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="4">

</xml_diff>